<commit_message>
make changes in captureTeamp test in WebApplicationTestCase class
</commit_message>
<xml_diff>
--- a/Framework/target/classes/com/ndtv/resources/TestData.xlsx
+++ b/Framework/target/classes/com/ndtv/resources/TestData.xlsx
@@ -33,13 +33,13 @@
     <t>APITestData</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>Allahabad</t>
   </si>
   <si>
     <t>http://api.openweathermap.org/data/2.5/weather</t>
+  </si>
+  <si>
+    <t>7fe67bf08c80ded756e598d6f8fedaea</t>
   </si>
 </sst>
 </file>
@@ -381,7 +381,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -405,13 +405,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>